<commit_message>
Up to date generator, started new documentation format
</commit_message>
<xml_diff>
--- a/data/testdata/SSG_LESSON_HOURS.xlsx
+++ b/data/testdata/SSG_LESSON_HOURS.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27002"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27511"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01B4BCDD-D11B-4A99-8D99-B6BDFEBA1706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{33B95735-9AC2-4718-BC9F-1B32AC82B69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>lesson_ID</t>
+    <t>lesson_id</t>
   </si>
   <si>
     <t>start_hour</t>
@@ -395,7 +395,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A15"/>
+      <selection activeCell="D2" sqref="D2:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -418,7 +418,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>0.3125</v>
@@ -429,7 +429,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>0.34722222222222227</v>
@@ -440,7 +440,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>0.38194444444444442</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>0.4201388888888889</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>0.4548611111111111</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>0.48958333333333331</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>0.52430555555555558</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>0.56944444444444442</v>
@@ -506,7 +506,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>0.60416666666666663</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>0.63888888888888895</v>
@@ -528,7 +528,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>0.67708333333333337</v>
@@ -539,7 +539,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>0.71527777777777779</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>0.75</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1">
         <v>0.78472222222222221</v>

</xml_diff>